<commit_message>
running with all data 2nd round
</commit_message>
<xml_diff>
--- a/data/img_labeling_2nd_round/missing.xlsx
+++ b/data/img_labeling_2nd_round/missing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>images</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>user</t>
-  </si>
-  <si>
-    <t>2058401-_providedCHO_fb5088d6_80da_05ab_8910_92bad635b6a6_1.jpeg</t>
-  </si>
-  <si>
-    <t>Yalemisew</t>
   </si>
 </sst>
 </file>
@@ -386,13 +380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,20 +397,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>